<commit_message>
commited by Swati on 20th May
</commit_message>
<xml_diff>
--- a/TestExecutor/src/main/resources/testData.xlsx
+++ b/TestExecutor/src/main/resources/testData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Enquero_Automation_Framework\TestExecutor\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SwatiChetty\TestAutomationFramework\TestExecutor\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0116FB-2F8A-4DBA-A2C0-8D9C869A0361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF4008A-9845-4CB2-9B94-952CD34324AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{03C0641D-4EAF-4ECB-AF6B-6704CD8ABCFB}"/>
   </bookViews>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>testLogin</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>InputParameters</t>
   </si>
@@ -44,9 +41,6 @@
     <t>ValidationParameters</t>
   </si>
   <si>
-    <t>testLoginFacebook</t>
-  </si>
-  <si>
     <t>TestCaseId</t>
   </si>
   <si>
@@ -69,6 +63,15 @@
   </si>
   <si>
     <t>{"textToValidate":"Order Create Successfully"}</t>
+  </si>
+  <si>
+    <t>testLoginJavascript</t>
+  </si>
+  <si>
+    <t>testLoginJasmine</t>
+  </si>
+  <si>
+    <t>testLoginSelenium</t>
   </si>
 </sst>
 </file>
@@ -420,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D1E5E7-639B-4CA4-9234-A0648C8A518A}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -436,44 +439,58 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -482,12 +499,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EF4EEBD71B7029418071E2948FBE3DFE" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2cd3803f1426b27e711f83538cce7781">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1dfacc6d-6701-4530-a587-2da6e9f4a883" xmlns:ns4="8ea24074-1ae4-4d8a-bed5-50beddb226f9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="953634c020f6c2985c7f3ba186b20de0" ns3:_="" ns4:_="">
     <xsd:import namespace="1dfacc6d-6701-4530-a587-2da6e9f4a883"/>
@@ -690,16 +716,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{521A633E-B03D-4D65-9917-E953736D8D12}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C234376-B86F-4B81-801E-F3A2527A814A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -716,7 +741,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FB56366-3CA6-44B6-BD76-738490901F6E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -733,12 +758,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{521A633E-B03D-4D65-9917-E953736D8D12}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>